<commit_message>
Completed putPlaylistMusic e putPlaylistMusic.
</commit_message>
<xml_diff>
--- a/PI WIKI.xlsx
+++ b/PI WIKI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luigi Sekuiya\Dropbox\ISEL - Trabalhos\PI - 1819v\Trabalho\PI-1819v-LI51N-G12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ECD624C-11AF-43AE-B950-0985DE0393B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0503DA8B-7F44-4507-9D96-D038F202BFAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18150" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <sheet name="Folha3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
   <si>
     <t>METHOD</t>
   </si>
@@ -272,6 +271,9 @@
   </si>
   <si>
     <t xml:space="preserve">    array</t>
+  </si>
+  <si>
+    <t>Mbid of the track</t>
   </si>
 </sst>
 </file>
@@ -832,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,21 +1437,33 @@
         <v>31</v>
       </c>
       <c r="I43" t="s">
+        <v>32</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G44" s="3"/>
+      <c r="H44" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I44" t="s">
         <v>30</v>
       </c>
-      <c r="J43" s="7" t="s">
+      <c r="J44" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G44" s="5"/>
-      <c r="H44" s="20" t="s">
+    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G45" s="5"/>
+      <c r="H45" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="I44" s="16" t="s">
+      <c r="I45" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J44" s="8" t="s">
+      <c r="J45" s="8" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug in yama-db in deletePlaylistMusic and putPlaylistMusic.
Fixed bug in yama-services.
Wiki updated.
</commit_message>
<xml_diff>
--- a/PI WIKI.xlsx
+++ b/PI WIKI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luigi Sekuiya\Dropbox\ISEL - Trabalhos\PI - 1819v\Trabalho\PI-1819v-LI51N-G12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bounty 34CE\Desktop\ISEL\PI\newStuff\PI-1819v-LI51N-G12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0503DA8B-7F44-4507-9D96-D038F202BFAF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A760F04-863C-4356-B6B6-B2E6F0ACC583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="20910" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
   <si>
     <t>METHOD</t>
   </si>
@@ -216,15 +216,6 @@
     <t>GetAlbum</t>
   </si>
   <si>
-    <t>GETARTIST</t>
-  </si>
-  <si>
-    <t>GetArtistTopAlbum</t>
-  </si>
-  <si>
-    <t>Request</t>
-  </si>
-  <si>
     <t>totalDuration</t>
   </si>
   <si>
@@ -274,6 +265,27 @@
   </si>
   <si>
     <t>Mbid of the track</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Collection of</t>
+  </si>
+  <si>
+    <t>Number of playlists</t>
+  </si>
+  <si>
+    <t>playlists</t>
+  </si>
+  <si>
+    <t>Array of PlaylistObjects</t>
+  </si>
+  <si>
+    <t>Playlist object editable information</t>
+  </si>
+  <si>
+    <t>GetArtistTopAlbums</t>
   </si>
 </sst>
 </file>
@@ -441,7 +453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -495,6 +507,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +868,7 @@
     <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
@@ -891,7 +912,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -911,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -991,7 +1012,7 @@
         <v>24</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H7" s="15"/>
     </row>
@@ -1023,16 +1044,16 @@
         <v>20</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1043,13 +1064,13 @@
         <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>19</v>
@@ -1058,7 +1079,7 @@
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="G12" s="23" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>28</v>
@@ -1128,7 +1149,7 @@
         <v>32</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="7:10" x14ac:dyDescent="0.25">
@@ -1156,7 +1177,7 @@
     <row r="20" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G20" s="3"/>
       <c r="H20" s="7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>45</v>
@@ -1168,7 +1189,7 @@
     <row r="21" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G21" s="3"/>
       <c r="H21" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>52</v>
@@ -1202,7 +1223,7 @@
         <v>32</v>
       </c>
       <c r="J23" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="7:10" x14ac:dyDescent="0.25">
@@ -1250,7 +1271,7 @@
         <v>32</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="7:10" x14ac:dyDescent="0.25">
@@ -1296,7 +1317,7 @@
         <v>32</v>
       </c>
       <c r="J31" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="7:10" x14ac:dyDescent="0.25">
@@ -1375,10 +1396,10 @@
         <v>33</v>
       </c>
       <c r="I38" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J38" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="7:10" x14ac:dyDescent="0.25">
@@ -1390,7 +1411,7 @@
         <v>30</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="7:10" x14ac:dyDescent="0.25">
@@ -1402,21 +1423,21 @@
         <v>41</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="7:10" x14ac:dyDescent="0.25">
       <c r="G41" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I41" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="7:10" x14ac:dyDescent="0.25">
@@ -1440,7 +1461,7 @@
         <v>32</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="7:10" x14ac:dyDescent="0.25">
@@ -1465,6 +1486,42 @@
       </c>
       <c r="J45" s="8" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G46" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="11"/>
+    </row>
+    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G48" s="5"/>
+      <c r="H48" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="I48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="J48" s="6" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Maybe done with artist tab.
</commit_message>
<xml_diff>
--- a/PI WIKI.xlsx
+++ b/PI WIKI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bounty 34CE\Desktop\ISEL\PI\newStuff\PI-1819v-LI51N-G12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mother Folder\Uni_shit\PI\PI-1819v-LI51N-G12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A760F04-863C-4356-B6B6-B2E6F0ACC583}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A08A8A0-D125-4F14-9A1B-4B54930A93D8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="13815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="720" windowWidth="19440" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="91">
   <si>
     <t>METHOD</t>
   </si>
@@ -75,9 +75,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>PARAMETERS</t>
-  </si>
-  <si>
     <t>/playlists</t>
   </si>
   <si>
@@ -286,6 +283,18 @@
   </si>
   <si>
     <t>GetArtistTopAlbums</t>
+  </si>
+  <si>
+    <t>/playlists/{pid}/track/music</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>String artist             String name</t>
+  </si>
+  <si>
+    <t>Query</t>
   </si>
 </sst>
 </file>
@@ -855,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J48"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,16 +875,16 @@
     <col min="1" max="1" width="10.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="11" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="11" max="12" width="44.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -886,16 +895,19 @@
         <v>1</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="E1" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>6</v>
       </c>
@@ -906,16 +918,19 @@
         <v>9</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -926,16 +941,19 @@
         <v>12</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
@@ -949,13 +967,16 @@
         <v>7</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
@@ -963,39 +984,45 @@
         <v>16</v>
       </c>
       <c r="C5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>15</v>
       </c>
@@ -1003,20 +1030,23 @@
         <v>5</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>15</v>
       </c>
@@ -1024,504 +1054,513 @@
         <v>5</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12"/>
-      <c r="G12" s="23" t="s">
+      <c r="H12" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H14" s="3"/>
+      <c r="I14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+      <c r="I17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="5"/>
+      <c r="I18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="10"/>
+      <c r="I19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="3"/>
+      <c r="I20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="3"/>
+      <c r="I21" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="3"/>
+      <c r="I24" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H25" s="3"/>
+      <c r="I25" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H26" s="3"/>
+      <c r="I26" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H27" s="5"/>
+      <c r="I27" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K27" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="10"/>
+      <c r="I28" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J28" s="21"/>
+      <c r="K28" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="3"/>
+      <c r="I29" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J29" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="3"/>
+      <c r="I30" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J30" t="s">
+        <v>54</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="3"/>
+      <c r="I31" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H32" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="3"/>
+      <c r="I33" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H34" s="3"/>
+      <c r="I34" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H35" s="3"/>
+      <c r="I35" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J35" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H36" s="5"/>
+      <c r="I36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K36" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H37" s="10"/>
+      <c r="I37" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="J37" s="21"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H38" s="3"/>
+      <c r="I38" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" t="s">
+        <v>75</v>
+      </c>
+      <c r="K38" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H39" s="3"/>
+      <c r="I39" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J39" t="s">
+        <v>29</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H40" s="3"/>
+      <c r="I40" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J40" t="s">
+        <v>40</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H41" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I41" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" t="s">
+        <v>63</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H42" s="3"/>
+      <c r="I42" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H43" s="3"/>
+      <c r="I43" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H44" s="3"/>
+      <c r="I44" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="J44" t="s">
+        <v>29</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H45" s="5"/>
+      <c r="I45" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="J45" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="K45" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H46" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="I46" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="J46" s="2"/>
+      <c r="K46" s="11"/>
+    </row>
+    <row r="47" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H47" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H48" s="5"/>
+      <c r="I48" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14" s="3"/>
-      <c r="H14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G15" s="12"/>
-      <c r="H15" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G16" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="3"/>
-      <c r="H17" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="5"/>
-      <c r="H18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="10"/>
-      <c r="H19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="3"/>
-      <c r="H20" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J20" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G21" s="3"/>
-      <c r="H21" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="3"/>
-      <c r="H24" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="3"/>
-      <c r="H25" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G26" s="3"/>
-      <c r="H26" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G27" s="5"/>
-      <c r="H27" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G28" s="10"/>
-      <c r="H28" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="I28" s="21"/>
-      <c r="J28" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G29" s="3"/>
-      <c r="H29" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I29" t="s">
-        <v>30</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G30" s="3"/>
-      <c r="H30" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I30" t="s">
-        <v>55</v>
-      </c>
-      <c r="J30" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G31" s="3"/>
-      <c r="H31" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" t="s">
-        <v>32</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G32" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H32" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" t="s">
-        <v>34</v>
-      </c>
-      <c r="J32" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G33" s="3"/>
-      <c r="H33" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I33" t="s">
-        <v>43</v>
-      </c>
-      <c r="J33" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G34" s="3"/>
-      <c r="H34" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I34" t="s">
-        <v>38</v>
-      </c>
-      <c r="J34" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G35" s="3"/>
-      <c r="H35" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G36" s="5"/>
-      <c r="H36" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G37" s="10"/>
-      <c r="H37" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G38" s="3"/>
-      <c r="H38" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I38" t="s">
-        <v>76</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G39" s="3"/>
-      <c r="H39" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I39" t="s">
-        <v>30</v>
-      </c>
-      <c r="J39" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="40" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G40" s="3"/>
-      <c r="H40" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="I40" t="s">
-        <v>41</v>
-      </c>
-      <c r="J40" s="7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G41" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="I41" t="s">
-        <v>64</v>
-      </c>
-      <c r="J41" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G42" s="3"/>
-      <c r="H42" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="I42" t="s">
-        <v>38</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G43" s="3"/>
-      <c r="H43" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I43" t="s">
-        <v>32</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G44" s="3"/>
-      <c r="H44" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="I44" t="s">
-        <v>30</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G45" s="5"/>
-      <c r="H45" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I45" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="J45" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G46" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H46" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="I46" s="2"/>
-      <c r="J46" s="11"/>
-    </row>
-    <row r="47" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G47" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H47" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="J47" s="4" t="s">
+      <c r="J48" s="8" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="48" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G48" s="5"/>
-      <c r="H48" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="I48" s="8" t="s">
+      <c r="K48" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>